<commit_message>
Adicoinado teste novo prompt
</commit_message>
<xml_diff>
--- a/dataframes/OMIEC_NEUROMORPHIC_RESPONSES.xlsx
+++ b/dataframes/OMIEC_NEUROMORPHIC_RESPONSES.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B45"/>
+  <dimension ref="A1:B55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,7 +451,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Conjugated polymers</t>
+          <t>PEDOT;poly(3,4-ethylenedioxythiophene)</t>
         </is>
       </c>
     </row>
@@ -461,7 +461,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Polymer-thiophene; poly(3,4-ethylenedioxythiophene) (PEDOT); polypyrrole; poly(3-hydroxybutyrate-co-3-hydroxyvalerate) (PHBV)</t>
+          <t>P(NDI2OD-T2F); PFO-NDC; PMEG; PNP2TP; poly(3,4-ethylenedioxythiophene) (PEDOT)</t>
         </is>
       </c>
     </row>
@@ -471,7 +471,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>organic semiconductor</t>
+          <t>PEDOT:PSS</t>
         </is>
       </c>
     </row>
@@ -481,7 +481,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Polymeriacs; Poly(3,4-ethylenedioxythiophene)</t>
+          <t>PEDOT:PSS</t>
         </is>
       </c>
     </row>
@@ -491,7 +491,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Polyaniline; Poly(3,4-ethylenedioxythiophene) (PEDOT); Poly(3,4-ethylenedioxythiophene)-poly(styrenesulfonate) (PEDOT:PSS)</t>
+          <t>P3HT</t>
         </is>
       </c>
     </row>
@@ -501,7 +501,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>PEDOT;Mel</t>
+          <t>DPEPH; MPyP; P(NTf2)3</t>
         </is>
       </c>
     </row>
@@ -511,7 +511,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>polythiophene; naphthalene diimide-based polymer</t>
+          <t>N,N'-Bis(3-methylphenyl)-3,4,9,10-perylene tetracarboxylic diimide (PTC); Active Layer Blend of Poly(ethylenedioxythiophene) (PEDOT) and Poly(styrenesulfonate) (PSS) (PEDOT:PSS)</t>
         </is>
       </c>
     </row>
@@ -521,7 +521,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Polymer names: Poly(3,4-ethylenedioxythiophene); Poly(3,4-ethylenedioxythiophene)-co-polystyrenesulfonate; None</t>
+          <t>Please input your text.</t>
         </is>
       </c>
     </row>
@@ -531,7 +531,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Poly(3,4-ethylenedioxythiophene); Poly-aniline; Poly(3,4-ethylenedioxythiophene)-poly(styrenesulfonate); P3HT; PEDOT-PSS.</t>
+          <t>P3HT; PEMA; Nafion</t>
         </is>
       </c>
     </row>
@@ -541,7 +541,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Polyvinylidene fluoride (PVDF); poly(3,4-ethylene dioxythiophene) (PEDOT); poly(3-hexylthiophene) (P3HT); polyurethane</t>
+          <t>Mel; PEDOT:PSS</t>
         </is>
       </c>
     </row>
@@ -551,7 +551,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>PEPDAT; PBTTTF</t>
         </is>
       </c>
     </row>
@@ -561,7 +561,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Polymer; Polyvinylidene fluoride (PVDF); Polypyrrole; Polyaniline; Polycarbonate; Polyethylene oxide; Polyethylene glycol; Poly 3-Hexylthiophene (P3HT); Poly(3,4-ethylenedioxythiophene) (PEDOT); Polymethyl methacrylate (PMMA); Poly(vinyl phenol) (PVPh)</t>
+          <t>PEDOT; PSS</t>
         </is>
       </c>
     </row>
@@ -571,7 +571,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Organic mixed ionic-electronic conducting polymer</t>
+          <t>NDI-2Tz; P-3O; P-4O; P-5O; P-6O</t>
         </is>
       </c>
     </row>
@@ -579,11 +579,7 @@
       <c r="A15" t="n">
         <v>13</v>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Poly(3,4-ethylenedioxythiophene)</t>
-        </is>
-      </c>
+      <c r="B15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -591,7 +587,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>PEDOT; PSS</t>
+          <t>P3MEEET</t>
         </is>
       </c>
     </row>
@@ -601,7 +597,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Conjugated polymers; Poly(3,4-ethylenedioxythiophene) (PEDOT); Poly(thiophene)</t>
+          <t>PEDOT:PSS; PSSNa</t>
         </is>
       </c>
     </row>
@@ -611,7 +607,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>PEDOT:PSS; P3HT</t>
         </is>
       </c>
     </row>
@@ -621,7 +617,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Poly(3,4-ethylenedioxythiophene)</t>
+          <t>PEDOT:PSS</t>
         </is>
       </c>
     </row>
@@ -631,7 +627,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>PEDOT:PSS</t>
+          <t>p(g2T-T); gDPP</t>
         </is>
       </c>
     </row>
@@ -641,7 +637,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>OMIEC</t>
+          <t>PEDOT; PSS</t>
         </is>
       </c>
     </row>
@@ -651,7 +647,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>P3MEEET</t>
+          <t>PEDOT-PSS; P3HT; PCBM</t>
         </is>
       </c>
     </row>
@@ -661,7 +657,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>NDI-2Tz copolymers; P-XO; P-6O</t>
+          <t>poly[4-ethoxythiophene] (PET); polythiophene (PT)</t>
         </is>
       </c>
     </row>
@@ -671,7 +667,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Polymer;</t>
+          <t>PEDOT;PSS</t>
         </is>
       </c>
     </row>
@@ -681,7 +677,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>PTCDA; P3HT</t>
         </is>
       </c>
     </row>
@@ -691,7 +687,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>TIIP;</t>
+          <t>DuPS-A; P(NDI2OD-T2); PFBT-Th</t>
         </is>
       </c>
     </row>
@@ -701,7 +697,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>PEDOT;PEDOT:PSS</t>
+          <t>PEDOT; PPy; PANI</t>
         </is>
       </c>
     </row>
@@ -711,7 +707,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>p(g2T-T); Homo-gDPP</t>
+          <t>PEDOT; PSS; Fenton's charge transfer complex; Nafion</t>
         </is>
       </c>
     </row>
@@ -721,7 +717,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Polythiophene;</t>
+          <t>oEG; P3HT</t>
         </is>
       </c>
     </row>
@@ -731,7 +727,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>P3HT; SEBS</t>
+          <t>PEDOT:PSS; PSSNa</t>
         </is>
       </c>
     </row>
@@ -741,7 +737,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>PCBM; C60-TEG</t>
+          <t>TIIP</t>
         </is>
       </c>
     </row>
@@ -751,7 +747,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Poly(vinylidenefluoride); poly(3,4-ethylenedioxythiophene); poly(3,4-ethylenedioxythiophene):poly(styrenesulfonate); polyanthrene; polypyrrole</t>
+          <t>P(NDI2OD-TSF-Br); P(NDI2OD-TNBT-Br); P(NDI2OD-TFB-Br</t>
         </is>
       </c>
     </row>
@@ -761,7 +757,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Polymers: None</t>
+          <t>PT; NDI</t>
         </is>
       </c>
     </row>
@@ -771,7 +767,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>P3HT;</t>
+          <t>PCBM; C60-TEG</t>
         </is>
       </c>
     </row>
@@ -781,7 +777,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>poly(vinylidene fluoride); poly(ethylene oxide); poly(3,4-ethylenedioxythiophene)</t>
+          <t>IMEIC; P3HT; PEDOT</t>
         </is>
       </c>
     </row>
@@ -791,7 +787,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Electrochromic polymers</t>
+          <t>PEDOT; PSS</t>
         </is>
       </c>
     </row>
@@ -801,7 +797,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>PIL; ion gel</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -811,7 +807,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>PEDOT:PSS</t>
+          <t>P3HT; SEBS</t>
         </is>
       </c>
     </row>
@@ -821,7 +817,8 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>PBBT; PBBT-Me; poly(benzimidazobenzophenanthroline) (BBL)</t>
+          <t>Poly-[N,N'-bis-(3-methylphenyl)-N,N'-bis(phenyl)-1,4-phenylenediamine]; 
+(Note: Please note that I've only extracted the OMIEC polymers mentioned in the text, which is Poly-[N,N'-bis-(3-methylphenyl)-N,N'-bis(phenyl)-1,4-phenylenediamine], which is commonly abbreviated as poly(NDI))</t>
         </is>
       </c>
     </row>
@@ -831,7 +828,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>polythiophene;oEG</t>
+          <t>PBedA;PFPDMA</t>
         </is>
       </c>
     </row>
@@ -841,7 +838,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>La2NiO4; P; Pt</t>
+          <t>PEDOT; PSS</t>
         </is>
       </c>
     </row>
@@ -851,7 +848,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>polythiophene</t>
+          <t>PEDOT:PSS</t>
         </is>
       </c>
     </row>
@@ -861,7 +858,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>PEDOT; PSS</t>
+          <t>Poly(3,4-ethylenedioxythiophene) (PEDOT); Poly(3-hexylthiophene) (P3HT)</t>
         </is>
       </c>
     </row>
@@ -871,7 +868,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Polymers used for neuromorphic devices: None</t>
+          <t>PEDOT; None</t>
         </is>
       </c>
     </row>
@@ -881,7 +878,107 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Polyaniline; Poly(3,4-ethylenedioxythiophene); None</t>
+          <t>P3MEEMT</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>PBBT; BBL</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>PEDOT:PSS</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>PEDOT:PSS</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>P(3HT), PEDOT:PSS</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>PSS; PDAC</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Polymer names: P3HT; PFS</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Adicionado NLP por tokenização e alguns testes por LLMs
</commit_message>
<xml_diff>
--- a/dataframes/OMIEC_NEUROMORPHIC_RESPONSES.xlsx
+++ b/dataframes/OMIEC_NEUROMORPHIC_RESPONSES.xlsx
@@ -451,7 +451,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>PEDOT;poly(3,4-ethylenedioxythiophene)</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -461,7 +461,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>P(NDI2OD-T2F); PFO-NDC; PMEG; PNP2TP; poly(3,4-ethylenedioxythiophene) (PEDOT)</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -471,7 +471,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>PEDOT:PSS</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -501,7 +501,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>DPEPH; MPyP; P(NTf2)3</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -511,7 +511,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>N,N'-Bis(3-methylphenyl)-3,4,9,10-perylene tetracarboxylic diimide (PTC); Active Layer Blend of Poly(ethylenedioxythiophene) (PEDOT) and Poly(styrenesulfonate) (PSS) (PEDOT:PSS)</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -521,7 +521,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Please input your text.</t>
+          <t>gNR-Bu</t>
         </is>
       </c>
     </row>
@@ -531,7 +531,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>P3HT; PEMA; Nafion</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -551,7 +551,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>PEPDAT; PBTTTF</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -561,7 +561,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>PEDOT; PSS</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -571,7 +571,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>NDI-2Tz; P-3O; P-4O; P-5O; P-6O</t>
+          <t>P-3O; P-4O; P-5O; P-6O</t>
         </is>
       </c>
     </row>
@@ -579,7 +579,11 @@
       <c r="A15" t="n">
         <v>13</v>
       </c>
-      <c r="B15" t="inlineStr"/>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -587,7 +591,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>P3MEEET</t>
+          <t>P3MEEET;</t>
         </is>
       </c>
     </row>
@@ -607,7 +611,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>PEDOT:PSS; P3HT</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -617,7 +621,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>PEDOT:PSS</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -627,7 +631,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>p(g2T-T); gDPP</t>
+          <t>p(g2T-T); Homo-gDPP</t>
         </is>
       </c>
     </row>
@@ -637,7 +641,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>PEDOT; PSS</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -647,7 +651,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>PEDOT-PSS; P3HT; PCBM</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -657,7 +661,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>poly[4-ethoxythiophene] (PET); polythiophene (PT)</t>
+          <t>PT-EG</t>
         </is>
       </c>
     </row>
@@ -667,7 +671,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>PEDOT;PSS</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -677,7 +681,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>PTCDA; P3HT</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -687,7 +691,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>DuPS-A; P(NDI2OD-T2); PFBT-Th</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -697,7 +701,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>PEDOT; PPy; PANI</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -707,7 +711,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>PEDOT; PSS; Fenton's charge transfer complex; Nafion</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -717,7 +721,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>oEG; P3HT</t>
+          <t>oEG-substituted polythiophene</t>
         </is>
       </c>
     </row>
@@ -727,7 +731,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>PEDOT:PSS; PSSNa</t>
+          <t>PEDOT:PSS</t>
         </is>
       </c>
     </row>
@@ -737,7 +741,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>TIIP</t>
+          <t>TIIP;</t>
         </is>
       </c>
     </row>
@@ -747,7 +751,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>P(NDI2OD-TSF-Br); P(NDI2OD-TNBT-Br); P(NDI2OD-TFB-Br</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -757,7 +761,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>PT; NDI</t>
+          <t>PT; NIDI</t>
         </is>
       </c>
     </row>
@@ -767,7 +771,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>PCBM; C60-TEG</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -777,7 +781,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>IMEIC; P3HT; PEDOT</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -787,7 +791,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>PEDOT; PSS</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -807,7 +811,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>P3HT; SEBS</t>
+          <t>P3HT</t>
         </is>
       </c>
     </row>
@@ -817,8 +821,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Poly-[N,N'-bis-(3-methylphenyl)-N,N'-bis(phenyl)-1,4-phenylenediamine]; 
-(Note: Please note that I've only extracted the OMIEC polymers mentioned in the text, which is Poly-[N,N'-bis-(3-methylphenyl)-N,N'-bis(phenyl)-1,4-phenylenediamine], which is commonly abbreviated as poly(NDI))</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -828,7 +831,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>PBedA;PFPDMA</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -838,7 +841,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>PEDOT; PSS</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -858,7 +861,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Poly(3,4-ethylenedioxythiophene) (PEDOT); Poly(3-hexylthiophene) (P3HT)</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -868,7 +871,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>PEDOT; None</t>
+          <t>PEDOT:PSS</t>
         </is>
       </c>
     </row>
@@ -888,7 +891,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>PBBT; BBL</t>
+          <t>PBBT-Me; BBL</t>
         </is>
       </c>
     </row>
@@ -928,7 +931,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>P(3HT), PEDOT:PSS</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -978,7 +981,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Polymer names: P3HT; PFS</t>
+          <t>None</t>
         </is>
       </c>
     </row>

</xml_diff>